<commit_message>
fixed glosses and add the missing sentence
</commit_message>
<xml_diff>
--- a/nar_RouDes_2017_04_26_002_yrk-tun.xlsx
+++ b/nar_RouDes_2017_04_26_002_yrk-tun.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Munkalap1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Munkalap1!$A$1:$J$193</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="385">
   <si>
     <t xml:space="preserve">Sent-Nr.</t>
   </si>
@@ -70,10 +73,10 @@
     <t xml:space="preserve">мар"</t>
   </si>
   <si>
-    <t xml:space="preserve">fence-gen.2sg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
+    <t xml:space="preserve">fence-gen.poss.2sg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOUN</t>
   </si>
   <si>
     <t xml:space="preserve">мюня</t>
@@ -82,7 +85,7 @@
     <t xml:space="preserve">behind</t>
   </si>
   <si>
-    <t xml:space="preserve">Adp</t>
+    <t xml:space="preserve">ADP</t>
   </si>
   <si>
     <t xml:space="preserve">нудм'.</t>
@@ -97,7 +100,7 @@
     <t xml:space="preserve">stand-1sg</t>
   </si>
   <si>
-    <t xml:space="preserve">V</t>
+    <t xml:space="preserve">VERB</t>
   </si>
   <si>
     <t xml:space="preserve">Маряд' мюня нум'.</t>
@@ -130,7 +133,7 @@
     <t xml:space="preserve">fence</t>
   </si>
   <si>
-    <t xml:space="preserve">нудм'</t>
+    <t xml:space="preserve">Нудм'.</t>
   </si>
   <si>
     <t xml:space="preserve">Тикахана сидя ты таняӈаха".</t>
@@ -151,7 +154,7 @@
     <t xml:space="preserve">there</t>
   </si>
   <si>
-    <t xml:space="preserve">Adv</t>
+    <t xml:space="preserve">ADV</t>
   </si>
   <si>
     <t xml:space="preserve">сидя</t>
@@ -160,7 +163,7 @@
     <t xml:space="preserve">two</t>
   </si>
   <si>
-    <t xml:space="preserve">Num</t>
+    <t xml:space="preserve">NUM</t>
   </si>
   <si>
     <t xml:space="preserve">ты</t>
@@ -262,7 +265,7 @@
     <t xml:space="preserve">сана-</t>
   </si>
   <si>
-    <t xml:space="preserve">jump-pfv.an-abl-obl.1sg</t>
+    <t xml:space="preserve">jump-pfv.an-abl-poss.1sg</t>
   </si>
   <si>
     <t xml:space="preserve">AN</t>
@@ -322,7 +325,7 @@
     <t xml:space="preserve">1sg.dat</t>
   </si>
   <si>
-    <t xml:space="preserve">Pron</t>
+    <t xml:space="preserve">PRON</t>
   </si>
   <si>
     <t xml:space="preserve">пирця</t>
@@ -331,7 +334,7 @@
     <t xml:space="preserve">tall</t>
   </si>
   <si>
-    <t xml:space="preserve">Adj</t>
+    <t xml:space="preserve">ADJ</t>
   </si>
   <si>
     <t xml:space="preserve">харадм'</t>
@@ -376,7 +379,7 @@
     <t xml:space="preserve">махалы</t>
   </si>
   <si>
-    <t xml:space="preserve">roof-3sg</t>
+    <t xml:space="preserve">roof-poss.3sg</t>
   </si>
   <si>
     <t xml:space="preserve">мятрев'</t>
@@ -418,7 +421,7 @@
     <t xml:space="preserve">сидер"</t>
   </si>
   <si>
-    <t xml:space="preserve">window-gen.3sg</t>
+    <t xml:space="preserve">window-gen.poss.3sg</t>
   </si>
   <si>
     <t xml:space="preserve">си,</t>
@@ -439,7 +442,7 @@
     <t xml:space="preserve">нё</t>
   </si>
   <si>
-    <t xml:space="preserve">door-gen.3sg</t>
+    <t xml:space="preserve">door-gen.poss.3sg</t>
   </si>
   <si>
     <t xml:space="preserve">таня.</t>
@@ -544,7 +547,7 @@
     <t xml:space="preserve">мя-т-тю-дм'</t>
   </si>
   <si>
-    <t xml:space="preserve">мят_тю-</t>
+    <t xml:space="preserve">мят-тю-</t>
   </si>
   <si>
     <t xml:space="preserve">enter-1sg</t>
@@ -796,7 +799,7 @@
     <t xml:space="preserve">ми-</t>
   </si>
   <si>
-    <t xml:space="preserve">go-ipfv.an-gen.1sg</t>
+    <t xml:space="preserve">go-ipfv.an-gen.poss.1sg</t>
   </si>
   <si>
     <t xml:space="preserve">яха'</t>
@@ -877,7 +880,7 @@
     <t xml:space="preserve">тарка-нда</t>
   </si>
   <si>
-    <t xml:space="preserve">fork-gen.3sg</t>
+    <t xml:space="preserve">fork-gen.poss.3sg</t>
   </si>
   <si>
     <t xml:space="preserve">пыя'</t>
@@ -931,7 +934,7 @@
     <t xml:space="preserve">мада-"ма-хада-ни'</t>
   </si>
   <si>
-    <t xml:space="preserve">pass.across-ipfv.an-abl-1sg</t>
+    <t xml:space="preserve">pass.across-ipfv.an-abl-poss.1sg</t>
   </si>
   <si>
     <t xml:space="preserve">ӈани'</t>
@@ -940,9 +943,6 @@
     <t xml:space="preserve">again</t>
   </si>
   <si>
-    <t xml:space="preserve">Cnj</t>
-  </si>
-  <si>
     <t xml:space="preserve">swim-cvb</t>
   </si>
   <si>
@@ -1027,7 +1027,7 @@
     <t xml:space="preserve">хэв</t>
   </si>
   <si>
-    <t xml:space="preserve">side-prol-3sg</t>
+    <t xml:space="preserve">side-prol-poss.3sg</t>
   </si>
   <si>
     <t xml:space="preserve">яля'</t>
@@ -1093,7 +1093,7 @@
     <t xml:space="preserve">яд-</t>
   </si>
   <si>
-    <t xml:space="preserve">walk-ipfv.an-gen.1sg</t>
+    <t xml:space="preserve">walk-ipfv.an-gen.poss.1sg</t>
   </si>
   <si>
     <t xml:space="preserve">пулм'</t>
@@ -1187,7 +1187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1210,30 +1210,25 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1284,7 +1279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1299,10 +1294,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1321,6 +1312,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1331,23 +1326,23 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="1" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="61.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1379,17 +1374,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1397,7 +1388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1414,8 +1405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1432,8 +1422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1450,20 +1439,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1471,7 +1453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1488,8 +1470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1506,8 +1487,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1524,23 +1504,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0"/>
       <c r="J12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1557,26 +1532,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="4" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1589,9 +1562,11 @@
       <c r="F15" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1604,9 +1579,12 @@
       <c r="F16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1624,9 +1602,8 @@
       <c r="I17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1643,24 +1620,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
       <c r="I20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1668,8 +1634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1686,8 +1651,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
@@ -1704,8 +1668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1722,8 +1685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1740,20 +1702,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
       <c r="I26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1761,7 +1716,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1778,8 +1733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1796,8 +1750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1814,8 +1767,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
         <v>64</v>
       </c>
@@ -1832,8 +1784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1850,8 +1801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
         <v>64</v>
       </c>
@@ -1868,8 +1818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
@@ -1886,8 +1835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
@@ -1904,20 +1852,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="0"/>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
-      <c r="F36" s="0"/>
       <c r="I36" s="1" t="s">
         <v>75</v>
       </c>
@@ -1925,7 +1866,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1941,11 +1882,11 @@
       <c r="G37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
         <v>82</v>
       </c>
@@ -1961,10 +1902,9 @@
       <c r="G38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
         <v>84</v>
       </c>
@@ -1981,8 +1921,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
         <v>68</v>
       </c>
@@ -1999,8 +1938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
         <v>87</v>
       </c>
@@ -2017,20 +1955,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="0"/>
-      <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="F43" s="0"/>
       <c r="I43" s="1" t="s">
         <v>92</v>
       </c>
@@ -2038,7 +1969,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
         <v>94</v>
       </c>
@@ -2055,8 +1986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
         <v>98</v>
       </c>
@@ -2073,8 +2003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
         <v>101</v>
       </c>
@@ -2091,8 +2020,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
         <v>104</v>
       </c>
@@ -2109,8 +2037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
         <v>108</v>
       </c>
@@ -2127,20 +2054,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
-      <c r="E50" s="0"/>
-      <c r="F50" s="0"/>
       <c r="I50" s="1" t="s">
         <v>113</v>
       </c>
@@ -2148,7 +2068,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
         <v>115</v>
       </c>
@@ -2165,8 +2085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
         <v>119</v>
       </c>
@@ -2183,8 +2102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="s">
         <v>123</v>
       </c>
@@ -2201,20 +2119,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="0"/>
-      <c r="D55" s="0"/>
-      <c r="E55" s="0"/>
-      <c r="F55" s="0"/>
       <c r="I55" s="1" t="s">
         <v>127</v>
       </c>
@@ -2222,7 +2133,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="1" t="s">
         <v>56</v>
       </c>
@@ -2239,8 +2150,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="1" t="s">
         <v>129</v>
       </c>
@@ -2257,8 +2167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
         <v>133</v>
       </c>
@@ -2275,8 +2184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
         <v>136</v>
       </c>
@@ -2293,8 +2201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
         <v>134</v>
       </c>
@@ -2311,8 +2218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="1" t="s">
         <v>140</v>
       </c>
@@ -2329,20 +2235,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C63" s="0"/>
-      <c r="D63" s="0"/>
-      <c r="E63" s="0"/>
-      <c r="F63" s="0"/>
       <c r="I63" s="1" t="s">
         <v>144</v>
       </c>
@@ -2350,7 +2249,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="1" t="s">
         <v>146</v>
       </c>
@@ -2367,8 +2266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="1" t="s">
         <v>134</v>
       </c>
@@ -2385,8 +2283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="1" t="s">
         <v>147</v>
       </c>
@@ -2403,20 +2300,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C68" s="0"/>
-      <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
       <c r="I68" s="1" t="s">
         <v>152</v>
       </c>
@@ -2424,7 +2314,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="1" t="s">
         <v>154</v>
       </c>
@@ -2441,8 +2331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
         <v>157</v>
       </c>
@@ -2459,8 +2348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
         <v>159</v>
       </c>
@@ -2477,20 +2365,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="0"/>
-      <c r="D73" s="0"/>
-      <c r="E73" s="0"/>
-      <c r="F73" s="0"/>
       <c r="I73" s="1" t="s">
         <v>164</v>
       </c>
@@ -2498,7 +2379,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="1" t="s">
         <v>166</v>
       </c>
@@ -2515,8 +2396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="1" t="s">
         <v>169</v>
       </c>
@@ -2533,8 +2413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="1" t="s">
         <v>172</v>
       </c>
@@ -2550,24 +2429,17 @@
       <c r="G76" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H76" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C78" s="0"/>
-      <c r="D78" s="0"/>
-      <c r="E78" s="0"/>
-      <c r="F78" s="0"/>
       <c r="I78" s="1" t="s">
         <v>178</v>
       </c>
@@ -2575,7 +2447,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="1" t="s">
         <v>180</v>
       </c>
@@ -2592,8 +2464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="1" t="s">
         <v>124</v>
       </c>
@@ -2610,8 +2481,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="1" t="s">
         <v>101</v>
       </c>
@@ -2628,8 +2498,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="1" t="s">
         <v>183</v>
       </c>
@@ -2646,8 +2515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="1" t="s">
         <v>186</v>
       </c>
@@ -2664,8 +2532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="1" t="s">
         <v>188</v>
       </c>
@@ -2682,8 +2549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="1" t="s">
         <v>190</v>
       </c>
@@ -2700,20 +2566,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C87" s="0"/>
-      <c r="D87" s="0"/>
-      <c r="E87" s="0"/>
-      <c r="F87" s="0"/>
       <c r="I87" s="1" t="s">
         <v>195</v>
       </c>
@@ -2721,7 +2580,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="1" t="s">
         <v>197</v>
       </c>
@@ -2738,8 +2597,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="1" t="s">
         <v>200</v>
       </c>
@@ -2756,20 +2614,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C91" s="0"/>
-      <c r="D91" s="0"/>
-      <c r="E91" s="0"/>
-      <c r="F91" s="0"/>
       <c r="I91" s="1" t="s">
         <v>205</v>
       </c>
@@ -2777,7 +2628,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
         <v>207</v>
       </c>
@@ -2794,8 +2645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="1" t="s">
         <v>210</v>
       </c>
@@ -2812,8 +2662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="1" t="s">
         <v>169</v>
       </c>
@@ -2830,8 +2679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="1" t="s">
         <v>211</v>
       </c>
@@ -2848,20 +2696,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="0"/>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C97" s="0"/>
-      <c r="D97" s="0"/>
-      <c r="E97" s="0"/>
-      <c r="F97" s="0"/>
       <c r="I97" s="1" t="s">
         <v>216</v>
       </c>
@@ -2869,7 +2710,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="1" t="s">
         <v>218</v>
       </c>
@@ -2886,8 +2727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="1" t="s">
         <v>219</v>
       </c>
@@ -2904,20 +2744,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0"/>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C101" s="0"/>
-      <c r="D101" s="0"/>
-      <c r="E101" s="0"/>
-      <c r="F101" s="0"/>
       <c r="I101" s="1" t="s">
         <v>224</v>
       </c>
@@ -2925,7 +2758,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="1" t="s">
         <v>166</v>
       </c>
@@ -2942,8 +2775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="1" t="s">
         <v>226</v>
       </c>
@@ -2960,8 +2792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="1" t="s">
         <v>229</v>
       </c>
@@ -2978,8 +2809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="1" t="s">
         <v>155</v>
       </c>
@@ -2996,8 +2826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="1" t="s">
         <v>157</v>
       </c>
@@ -3014,8 +2843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="0"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="1" t="s">
         <v>233</v>
       </c>
@@ -3032,20 +2860,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="0"/>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C109" s="0"/>
-      <c r="D109" s="0"/>
-      <c r="E109" s="0"/>
-      <c r="F109" s="0"/>
       <c r="I109" s="1" t="s">
         <v>238</v>
       </c>
@@ -3053,7 +2874,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="1" t="s">
         <v>240</v>
       </c>
@@ -3070,8 +2891,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0"/>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="1" t="s">
         <v>241</v>
       </c>
@@ -3088,8 +2908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="1" t="s">
         <v>243</v>
       </c>
@@ -3106,8 +2925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="0"/>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="1" t="s">
         <v>245</v>
       </c>
@@ -3124,20 +2942,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="0"/>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C115" s="0"/>
-      <c r="D115" s="0"/>
-      <c r="E115" s="0"/>
-      <c r="F115" s="0"/>
       <c r="I115" s="1" t="s">
         <v>250</v>
       </c>
@@ -3145,7 +2956,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="1" t="s">
         <v>252</v>
       </c>
@@ -3162,8 +2973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="0"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="1" t="s">
         <v>255</v>
       </c>
@@ -3179,12 +2989,11 @@
       <c r="G117" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H117" s="5" t="s">
+      <c r="H117" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0"/>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="1" t="s">
         <v>157</v>
       </c>
@@ -3201,8 +3010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="0"/>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="1" t="s">
         <v>259</v>
       </c>
@@ -3219,8 +3027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="0"/>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="1" t="s">
         <v>263</v>
       </c>
@@ -3237,8 +3044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="0"/>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="1" t="s">
         <v>267</v>
       </c>
@@ -3255,20 +3061,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="0"/>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C123" s="0"/>
-      <c r="D123" s="0"/>
-      <c r="E123" s="0"/>
-      <c r="F123" s="0"/>
       <c r="I123" s="1" t="s">
         <v>272</v>
       </c>
@@ -3276,7 +3075,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="1" t="s">
         <v>207</v>
       </c>
@@ -3293,8 +3092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="0"/>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="1" t="s">
         <v>259</v>
       </c>
@@ -3311,8 +3109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="0"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="1" t="s">
         <v>274</v>
       </c>
@@ -3329,8 +3126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="0"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="1" t="s">
         <v>277</v>
       </c>
@@ -3346,12 +3142,11 @@
       <c r="G127" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H127" s="5" t="s">
+      <c r="H127" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="0"/>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="1" t="s">
         <v>200</v>
       </c>
@@ -3368,20 +3163,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="0"/>
-    </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C130" s="0"/>
-      <c r="D130" s="0"/>
-      <c r="E130" s="0"/>
-      <c r="F130" s="0"/>
       <c r="I130" s="1" t="s">
         <v>281</v>
       </c>
@@ -3389,7 +3177,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="1" t="s">
         <v>283</v>
       </c>
@@ -3406,8 +3194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="0"/>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="1" t="s">
         <v>286</v>
       </c>
@@ -3424,8 +3211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="0"/>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="1" t="s">
         <v>290</v>
       </c>
@@ -3442,8 +3228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="0"/>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="1" t="s">
         <v>159</v>
       </c>
@@ -3460,20 +3245,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="0"/>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C136" s="0"/>
-      <c r="D136" s="0"/>
-      <c r="E136" s="0"/>
-      <c r="F136" s="0"/>
       <c r="I136" s="1" t="s">
         <v>296</v>
       </c>
@@ -3481,7 +3259,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="1" t="s">
         <v>283</v>
       </c>
@@ -3498,8 +3276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="0"/>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="1" t="s">
         <v>298</v>
       </c>
@@ -3516,8 +3293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="0"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="1" t="s">
         <v>301</v>
       </c>
@@ -3533,12 +3309,11 @@
       <c r="G139" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H139" s="5" t="s">
+      <c r="H139" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="0"/>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="1" t="s">
         <v>304</v>
       </c>
@@ -3552,11 +3327,10 @@
         <v>305</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="1" t="s">
         <v>277</v>
       </c>
@@ -3567,17 +3341,16 @@
         <v>277</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H141" s="5" t="s">
+      <c r="H141" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="0"/>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="1" t="s">
         <v>241</v>
       </c>
@@ -3594,25 +3367,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="0"/>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>261</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="1" t="s">
         <v>200</v>
       </c>
@@ -3629,43 +3401,38 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B146" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I146" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C146" s="0"/>
-      <c r="D146" s="0"/>
-      <c r="E146" s="0"/>
-      <c r="F146" s="0"/>
-      <c r="I146" s="1" t="s">
+      <c r="J146" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="J146" s="1" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E147" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F147" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="0"/>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="1" t="s">
         <v>304</v>
       </c>
@@ -3679,32 +3446,30 @@
         <v>305</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="E149" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="F149" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F149" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="G149" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H149" s="5" t="s">
+      <c r="H149" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="0"/>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="1" t="s">
         <v>96</v>
       </c>
@@ -3721,8 +3486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="0"/>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="1" t="s">
         <v>98</v>
       </c>
@@ -3739,25 +3503,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="0"/>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="E152" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="F152" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F152" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="G152" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="1" t="s">
         <v>108</v>
       </c>
@@ -3774,151 +3537,139 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I155" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C155" s="0"/>
-      <c r="D155" s="0"/>
-      <c r="E155" s="0"/>
-      <c r="F155" s="0"/>
-      <c r="I155" s="1" t="s">
+      <c r="J155" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="J155" s="1" t="s">
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="1" t="s">
+      <c r="D156" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="0"/>
-      <c r="C157" s="1" t="s">
+      <c r="D157" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E157" s="1" t="s">
+      <c r="F157" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="0"/>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="G158" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="G158" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="0"/>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E159" s="1" t="s">
+      <c r="F159" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="F159" s="1" t="s">
+      <c r="G159" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="G159" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="0"/>
-      <c r="C160" s="1" t="s">
+      <c r="D160" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F160" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>341</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D161" s="1" t="s">
+      <c r="E161" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="F161" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F161" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="G161" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B163" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="I163" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C163" s="0"/>
-      <c r="D163" s="0"/>
-      <c r="E163" s="0"/>
-      <c r="F163" s="0"/>
-      <c r="I163" s="1" t="s">
+      <c r="J163" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="J163" s="1" t="s">
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="1" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>84</v>
@@ -3933,16 +3684,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="0"/>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>86</v>
@@ -3951,46 +3701,44 @@
         <v>43</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="0"/>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="E166" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F166" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="G166" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="0"/>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="E167" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="F167" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="F167" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G167" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H167" s="5" t="s">
+      <c r="H167" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="1" t="s">
         <v>157</v>
       </c>
@@ -4007,24 +3755,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="F169" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="F169" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="G169" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="1" t="s">
         <v>108</v>
       </c>
@@ -4041,43 +3789,38 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B172" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="I172" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C172" s="0"/>
-      <c r="D172" s="0"/>
-      <c r="E172" s="0"/>
-      <c r="F172" s="0"/>
-      <c r="I172" s="1" t="s">
+      <c r="J172" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="J172" s="1" t="s">
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D173" s="1" t="s">
+      <c r="E173" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F173" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E173" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>367</v>
-      </c>
       <c r="G173" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="0"/>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="1" t="s">
         <v>157</v>
       </c>
@@ -4094,30 +3837,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="0"/>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C175" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D175" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>261</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>208</v>
@@ -4129,7 +3871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="1" t="s">
         <v>62</v>
       </c>
@@ -4140,13 +3882,13 @@
         <v>62</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C178" s="1" t="s">
         <v>200</v>
       </c>
@@ -4163,80 +3905,75 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B180" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="I180" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C180" s="0"/>
-      <c r="D180" s="0"/>
-      <c r="E180" s="0"/>
-      <c r="F180" s="0"/>
-      <c r="I180" s="1" t="s">
+      <c r="J180" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="J180" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D181" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="E181" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F181" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="0"/>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D182" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="E182" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="F182" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="F182" s="1" t="s">
+      <c r="G182" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C183" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="G182" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>247</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H183" s="5" t="s">
+      <c r="H183" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="1" t="s">
         <v>84</v>
       </c>
@@ -4253,7 +3990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C185" s="1" t="s">
         <v>68</v>
       </c>
@@ -4270,59 +4007,55 @@
         <v>43</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D186" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F186" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B188" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I188" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C188" s="0"/>
-      <c r="D188" s="0"/>
-      <c r="E188" s="0"/>
-      <c r="F188" s="0"/>
-      <c r="I188" s="1" t="s">
+      <c r="J188" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="J188" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D189" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D189" s="1" t="s">
+      <c r="E189" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F189" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="1" t="s">
         <v>64</v>
       </c>
@@ -4339,7 +4072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="1" t="s">
         <v>138</v>
       </c>
@@ -4350,13 +4083,13 @@
         <v>138</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C192" s="1" t="s">
         <v>169</v>
       </c>
@@ -4373,7 +4106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="1" t="s">
         <v>211</v>
       </c>
@@ -4384,21 +4117,15 @@
         <v>213</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G193" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:J193"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4406,5 +4133,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Oldal &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>